<commit_message>
Added Script Path allow list support to exclusion import
</commit_message>
<xml_diff>
--- a/tanium_exclusions.xlsx
+++ b/tanium_exclusions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrick.v\Desktop\code\deepinstinct-rest-api-wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB95AB4F-1D7F-4DA5-A990-EC94095F4082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178B3566-D5CF-4D8F-95B8-7E67AA2CE2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="972" yWindow="4812" windowWidth="21276" windowHeight="18576" xr2:uid="{2BD41A49-0820-434A-A6DC-4D89221EB3A9}"/>
   </bookViews>
@@ -595,9 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D56C3A-A8A5-43A1-9EFD-4D48E4663CEA}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>